<commit_message>
DC : Updated time sheet
</commit_message>
<xml_diff>
--- a/documentation/Timesheets/Timesheet Dave Cloete.xlsx
+++ b/documentation/Timesheets/Timesheet Dave Cloete.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Matsobane Khwinana" sheetId="1" r:id="rId1"/>
+    <sheet name="Dave Cloete" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -59,33 +59,12 @@
     <t>Project Group Meeting 5</t>
   </si>
   <si>
-    <t>Duration Hours</t>
-  </si>
-  <si>
-    <t>UI POC: D3 Charting - Globe chart</t>
-  </si>
-  <si>
-    <t>UI POC: Node.js static web and controllers</t>
-  </si>
-  <si>
-    <t>UI: Started with world /state Maps</t>
-  </si>
-  <si>
     <t>Project Group Meeting 6</t>
   </si>
   <si>
     <t>Project Group Meeting 7</t>
   </si>
   <si>
-    <t>UI: Criteria Configuration</t>
-  </si>
-  <si>
-    <t>UI: Initial Stream Graphs</t>
-  </si>
-  <si>
-    <t>UI POC: More work on Node.js Controllers. Added twig templating</t>
-  </si>
-  <si>
     <t>UI POC: D3 charting - Bar Chart tutorial, customised V Bar chart</t>
   </si>
   <si>
@@ -95,15 +74,6 @@
     <t xml:space="preserve">UI POC: D3 charting - Heat Maps (Days/months) + refactoring of </t>
   </si>
   <si>
-    <t>UI POC: Testing and Minor tweaking</t>
-  </si>
-  <si>
-    <t>UI: Finish off Heat maps V1</t>
-  </si>
-  <si>
-    <t>UI: Stream Graphs</t>
-  </si>
-  <si>
     <t>Project Group Meeting 8</t>
   </si>
   <si>
@@ -114,6 +84,48 @@
   </si>
   <si>
     <t>Reports - Individual and Group &amp; Group Meeting 11(Virtual)</t>
+  </si>
+  <si>
+    <t>Project Group Meeting 12</t>
+  </si>
+  <si>
+    <t>Actual Hours</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
+  </si>
+  <si>
+    <t>UI: Stream Graphs - Part 1</t>
+  </si>
+  <si>
+    <t>UI: Stream Graphs - Part 2</t>
+  </si>
+  <si>
+    <t>UI: Initial Stream Graph Research</t>
+  </si>
+  <si>
+    <t>UI: Criteria Configuration - Part 1</t>
+  </si>
+  <si>
+    <t>UI: Criteria Configuration - Part 2</t>
+  </si>
+  <si>
+    <t>UI: World /state Maps - Part 1</t>
+  </si>
+  <si>
+    <t>UI POC: Refactor and Testing</t>
+  </si>
+  <si>
+    <t>UI POC: Node.js Static web and Controllers</t>
+  </si>
+  <si>
+    <t>UI POC: Node.js Controllers - Added twig templating</t>
+  </si>
+  <si>
+    <t>UI POC: D3 Charting - Globe Chart</t>
+  </si>
+  <si>
+    <t>UI: Heat maps - Final</t>
   </si>
 </sst>
 </file>
@@ -201,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -211,8 +223,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -573,11 +616,12 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.42578125"/>
+    <col min="5" max="5" width="15.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="1026" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -585,8 +629,9 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,11 +644,14 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -616,12 +664,15 @@
       <c r="D3" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E3" s="4">
-        <f t="shared" ref="E3:E44" si="0">D3-C3</f>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="14">
+        <f t="shared" ref="E3:F44" si="0">D3-C3</f>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -634,14 +685,17 @@
       <c r="D4" s="4">
         <v>0.875</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3">
         <v>42491</v>
@@ -652,12 +706,15 @@
       <c r="D5" s="4">
         <v>0.5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="8">
+        <v>2</v>
+      </c>
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -670,14 +727,17 @@
       <c r="D6" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3">
         <v>42493</v>
@@ -688,14 +748,17 @@
       <c r="D7" s="5">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="9">
+        <v>4</v>
+      </c>
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>0.20833333333333359</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3">
         <v>42497</v>
@@ -706,12 +769,15 @@
       <c r="D8" s="4">
         <v>0.625</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>0.20833333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -724,14 +790,17 @@
       <c r="D9" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>42504</v>
@@ -742,12 +811,15 @@
       <c r="D10" s="4">
         <v>0.75</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -760,14 +832,17 @@
       <c r="D11" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="8">
+        <v>2</v>
+      </c>
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>42506</v>
@@ -778,14 +853,17 @@
       <c r="D12" s="4">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="8">
+        <v>4</v>
+      </c>
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666674</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3">
         <v>42511</v>
@@ -796,12 +874,15 @@
       <c r="D13" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="8">
+        <v>4</v>
+      </c>
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -814,14 +895,17 @@
       <c r="D14" s="4">
         <v>0.6875</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>42512</v>
@@ -832,14 +916,17 @@
       <c r="D15" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3">
         <v>42518</v>
@@ -850,14 +937,17 @@
       <c r="D16" s="4">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="8">
+        <v>8</v>
+      </c>
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3">
         <v>42525</v>
@@ -868,14 +958,17 @@
       <c r="D17" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="8">
+        <v>2</v>
+      </c>
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3">
         <v>42526</v>
@@ -886,14 +979,17 @@
       <c r="D18" s="4">
         <v>0.75</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B19" s="3">
         <v>42529</v>
@@ -904,14 +1000,17 @@
       <c r="D19" s="4">
         <v>0.91666666666666663</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="8">
+        <v>2</v>
+      </c>
+      <c r="F19" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="3">
         <v>42532</v>
@@ -922,14 +1021,17 @@
       <c r="D20" s="4">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="8">
+        <v>2</v>
+      </c>
+      <c r="F20" s="14">
         <f t="shared" si="0"/>
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3">
         <v>42533</v>
@@ -940,14 +1042,17 @@
       <c r="D21" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="8">
+        <v>4</v>
+      </c>
+      <c r="F21" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666674</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>42535</v>
@@ -958,14 +1063,17 @@
       <c r="D22" s="4">
         <v>0.95833333333333337</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="8">
+        <v>4</v>
+      </c>
+      <c r="F22" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666674</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
         <v>42537</v>
@@ -976,14 +1084,17 @@
       <c r="D23" s="4">
         <v>0.75</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="8">
+        <v>4</v>
+      </c>
+      <c r="F23" s="14">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3">
         <v>42538</v>
@@ -994,14 +1105,17 @@
       <c r="D24" s="4">
         <v>0.5</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="8">
+        <v>4</v>
+      </c>
+      <c r="F24" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666669</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3">
         <v>42539</v>
@@ -1012,14 +1126,17 @@
       <c r="D25" s="4">
         <v>0.875</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="8">
+        <v>8</v>
+      </c>
+      <c r="F25" s="14">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B26" s="3">
         <v>42540</v>
@@ -1030,14 +1147,17 @@
       <c r="D26" s="4">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="8">
+        <v>2</v>
+      </c>
+      <c r="F26" s="14">
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B27" s="3">
         <v>42547</v>
@@ -1048,14 +1168,17 @@
       <c r="D27" s="4">
         <v>0.72916666666666663</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="8">
+        <v>2</v>
+      </c>
+      <c r="F27" s="14">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3">
         <v>42551</v>
@@ -1066,184 +1189,217 @@
       <c r="D28" s="4">
         <v>0.77083333333333337</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="8">
+        <v>8</v>
+      </c>
+      <c r="F28" s="14">
         <f t="shared" si="0"/>
         <v>0.39583333333333337</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="3">
+        <v>42552</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E29" s="8">
+        <v>8</v>
+      </c>
+      <c r="F29" s="14">
+        <f t="shared" si="0"/>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="9"/>
+      <c r="F30" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="9"/>
+      <c r="F31" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="9"/>
+      <c r="F32" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E33" s="9"/>
+      <c r="F33" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E34" s="9"/>
+      <c r="F34" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="9"/>
+      <c r="F35" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E36" s="9"/>
+      <c r="F36" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="9"/>
+      <c r="F37" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E38" s="9"/>
+      <c r="F38" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" s="9"/>
+      <c r="F39" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E40" s="9"/>
+      <c r="F40" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E41" s="9"/>
+      <c r="F41" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="9"/>
+      <c r="F42" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E43" s="9"/>
+      <c r="F43" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
-      <c r="E44" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="8">
+      <c r="E44" s="10"/>
+      <c r="F44" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="11">
         <f>SUM(E3:E44)</f>
-        <v>4.9375000000000009</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+        <v>96</v>
+      </c>
+      <c r="F45" s="16">
+        <f>SUM(F3:F44)</f>
+        <v>5.2291666666666679</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>